<commit_message>
Contact Module Test Cases Done EventFire Added Extent Report Implement
</commit_message>
<xml_diff>
--- a/CLXTest/src/main/java/com/clx/qa/testdata/CLXTestData.xlsx
+++ b/CLXTest/src/main/java/com/clx/qa/testdata/CLXTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Specility</t>
   </si>
@@ -45,19 +45,67 @@
     <t>CLX</t>
   </si>
   <si>
-    <t>Dhiraj</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Redekar</t>
-  </si>
-  <si>
     <t>dredekar@yopmail.com</t>
   </si>
   <si>
     <t>(852) 336-6654</t>
+  </si>
+  <si>
+    <t>Ned</t>
+  </si>
+  <si>
+    <t>New Park</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>New Park New Way</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>New City</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>234-234-234234</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Eddard</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Luiz</t>
+  </si>
+  <si>
+    <t>Client</t>
   </si>
 </sst>
 </file>
@@ -102,9 +150,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,98 +459,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2">
+        <v>22222</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2">
+        <v>22222</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>